<commit_message>
changeover times per line from input
</commit_message>
<xml_diff>
--- a/InputCMPC 3.xlsx
+++ b/InputCMPC 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68244661-FD9D-4458-8BDE-99216ED9EFA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB10D94F-B015-44F2-86F6-3E597FB8E915}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Lines" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SKU!$A$1:$M$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SKU!$A$1:$L$97</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="63">
   <si>
     <t>100-AAA-04-016</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>country_demand</t>
-  </si>
-  <si>
-    <t>pro_price</t>
   </si>
   <si>
     <t>Argentina</t>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t>fte</t>
+  </si>
+  <si>
+    <t>co_size_time</t>
+  </si>
+  <si>
+    <t>co_packsize_time</t>
   </si>
 </sst>
 </file>
@@ -1216,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1232,15 +1235,14 @@
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="6.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1266,19 +1268,19 @@
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L1" t="s">
         <v>48</v>
       </c>
       <c r="M1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="N1" t="s">
         <v>42</v>
@@ -1295,11 +1297,8 @@
       <c r="R1" t="s">
         <v>46</v>
       </c>
-      <c r="S1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,11 +1323,11 @@
       <c r="H2">
         <v>119.42400000000001</v>
       </c>
-      <c r="I2">
-        <v>0.4163</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
       </c>
       <c r="K2" s="3">
         <v>0</v>
@@ -1337,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N2" s="3">
         <v>800</v>
@@ -1354,11 +1353,8 @@
       <c r="R2" s="3">
         <v>800</v>
       </c>
-      <c r="S2" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,11 +1379,11 @@
       <c r="H3">
         <v>204.16</v>
       </c>
-      <c r="I3">
-        <v>0.4163</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
@@ -1396,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N3" s="3">
         <v>800</v>
@@ -1413,11 +1409,8 @@
       <c r="R3" s="3">
         <v>800</v>
       </c>
-      <c r="S3" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,11 +1435,11 @@
       <c r="H4">
         <v>298.45301799999999</v>
       </c>
-      <c r="I4">
-        <v>0.4163</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
       </c>
       <c r="K4" s="3">
         <v>0</v>
@@ -1455,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N4" s="3">
         <v>800</v>
@@ -1472,11 +1465,8 @@
       <c r="R4" s="3">
         <v>800</v>
       </c>
-      <c r="S4" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1501,11 +1491,11 @@
       <c r="H5">
         <v>211.46789711111109</v>
       </c>
-      <c r="I5">
-        <v>0.4163</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
       </c>
       <c r="K5" s="3">
         <v>0</v>
@@ -1514,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N5" s="3">
         <v>800</v>
@@ -1531,11 +1521,8 @@
       <c r="R5" s="3">
         <v>800</v>
       </c>
-      <c r="S5" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,11 +1547,11 @@
       <c r="H6">
         <v>219.27742211111109</v>
       </c>
-      <c r="I6">
-        <v>0.4163</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
       </c>
       <c r="K6" s="3">
         <v>0</v>
@@ -1573,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N6" s="3">
         <v>800</v>
@@ -1590,11 +1577,8 @@
       <c r="R6" s="3">
         <v>800</v>
       </c>
-      <c r="S6" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1619,11 +1603,11 @@
       <c r="H7">
         <v>218.85455444444443</v>
       </c>
-      <c r="I7">
-        <v>0.4163</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
       </c>
       <c r="K7" s="3">
         <v>0</v>
@@ -1632,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N7" s="3">
         <v>800</v>
@@ -1649,11 +1633,8 @@
       <c r="R7" s="3">
         <v>800</v>
       </c>
-      <c r="S7" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1678,11 +1659,11 @@
       <c r="H8">
         <v>188.59963044444444</v>
       </c>
-      <c r="I8">
-        <v>0.4163</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
       </c>
       <c r="K8" s="3">
         <v>0</v>
@@ -1691,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N8" s="3">
         <v>800</v>
@@ -1708,11 +1689,8 @@
       <c r="R8" s="3">
         <v>800</v>
       </c>
-      <c r="S8" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1737,11 +1715,11 @@
       <c r="H9">
         <v>190.8653332222222</v>
       </c>
-      <c r="I9">
-        <v>0.4163</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
       </c>
       <c r="K9" s="3">
         <v>0</v>
@@ -1750,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N9" s="3">
         <v>800</v>
@@ -1767,11 +1745,8 @@
       <c r="R9" s="3">
         <v>800</v>
       </c>
-      <c r="S9" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1796,11 +1771,11 @@
       <c r="H10">
         <v>173.11802111111109</v>
       </c>
-      <c r="I10">
-        <v>0.4163</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
@@ -1809,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N10" s="3">
         <v>800</v>
@@ -1826,11 +1801,8 @@
       <c r="R10" s="3">
         <v>800</v>
       </c>
-      <c r="S10" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1855,11 +1827,11 @@
       <c r="H11">
         <v>187.93370577892941</v>
       </c>
-      <c r="I11">
-        <v>0.4163</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
       </c>
       <c r="K11" s="3">
         <v>0</v>
@@ -1868,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N11" s="3">
         <v>800</v>
@@ -1885,11 +1857,8 @@
       <c r="R11" s="3">
         <v>800</v>
       </c>
-      <c r="S11" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,11 +1883,11 @@
       <c r="H12">
         <v>306.08259578212858</v>
       </c>
-      <c r="I12">
-        <v>0.4163</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
       </c>
       <c r="K12" s="3">
         <v>0</v>
@@ -1927,7 +1896,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N12" s="3">
         <v>800</v>
@@ -1944,11 +1913,8 @@
       <c r="R12" s="3">
         <v>800</v>
       </c>
-      <c r="S12" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1973,11 +1939,11 @@
       <c r="H13">
         <v>198.93099661647744</v>
       </c>
-      <c r="I13">
-        <v>0.4163</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
       </c>
       <c r="K13" s="3">
         <v>0</v>
@@ -1986,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N13" s="3">
         <v>800</v>
@@ -2003,11 +1969,8 @@
       <c r="R13" s="3">
         <v>800</v>
       </c>
-      <c r="S13" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2032,11 +1995,11 @@
       <c r="H14">
         <v>85.12</v>
       </c>
-      <c r="I14">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
@@ -2045,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N14" s="3">
         <v>800</v>
@@ -2062,11 +2025,8 @@
       <c r="R14" s="3">
         <v>800</v>
       </c>
-      <c r="S14" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -2091,11 +2051,11 @@
       <c r="H15">
         <v>172.32</v>
       </c>
-      <c r="I15">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1</v>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
       </c>
       <c r="K15" s="3">
         <v>0</v>
@@ -2104,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N15" s="3">
         <v>800</v>
@@ -2121,11 +2081,8 @@
       <c r="R15" s="3">
         <v>800</v>
       </c>
-      <c r="S15" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2150,11 +2107,11 @@
       <c r="H16">
         <v>300.01198299999999</v>
       </c>
-      <c r="I16">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1</v>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
@@ -2163,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N16" s="3">
         <v>800</v>
@@ -2180,11 +2137,8 @@
       <c r="R16" s="3">
         <v>800</v>
       </c>
-      <c r="S16" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2209,11 +2163,11 @@
       <c r="H17">
         <v>186.79569833333329</v>
       </c>
-      <c r="I17">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1</v>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
       </c>
       <c r="K17" s="3">
         <v>0</v>
@@ -2222,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N17" s="3">
         <v>800</v>
@@ -2239,11 +2193,8 @@
       <c r="R17" s="3">
         <v>800</v>
       </c>
-      <c r="S17" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -2268,11 +2219,11 @@
       <c r="H18">
         <v>206.99054833333332</v>
       </c>
-      <c r="I18">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1</v>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
@@ -2281,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N18" s="3">
         <v>800</v>
@@ -2298,11 +2249,8 @@
       <c r="R18" s="3">
         <v>800</v>
       </c>
-      <c r="S18" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2327,11 +2275,11 @@
       <c r="H19">
         <v>178.69372433333336</v>
       </c>
-      <c r="I19">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J19" s="2">
-        <v>1</v>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
       </c>
       <c r="K19" s="3">
         <v>0</v>
@@ -2340,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N19" s="3">
         <v>800</v>
@@ -2357,11 +2305,8 @@
       <c r="R19" s="3">
         <v>800</v>
       </c>
-      <c r="S19" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2386,11 +2331,11 @@
       <c r="H20">
         <v>162.21178833333332</v>
       </c>
-      <c r="I20">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1</v>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
@@ -2399,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N20" s="3">
         <v>800</v>
@@ -2416,11 +2361,8 @@
       <c r="R20" s="3">
         <v>800</v>
       </c>
-      <c r="S20" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2445,11 +2387,11 @@
       <c r="H21">
         <v>150.17341066666665</v>
       </c>
-      <c r="I21">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1</v>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
       </c>
       <c r="K21" s="3">
         <v>0</v>
@@ -2458,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N21" s="3">
         <v>800</v>
@@ -2475,11 +2417,8 @@
       <c r="R21" s="3">
         <v>800</v>
       </c>
-      <c r="S21" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -2504,11 +2443,11 @@
       <c r="H22">
         <v>142.49757633333334</v>
       </c>
-      <c r="I22">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J22" s="2">
-        <v>1</v>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
@@ -2517,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N22" s="3">
         <v>800</v>
@@ -2534,11 +2473,8 @@
       <c r="R22" s="3">
         <v>800</v>
       </c>
-      <c r="S22" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -2563,11 +2499,11 @@
       <c r="H23">
         <v>207.41980332740238</v>
       </c>
-      <c r="I23">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
       </c>
       <c r="K23" s="3">
         <v>0</v>
@@ -2576,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N23" s="3">
         <v>800</v>
@@ -2593,11 +2529,8 @@
       <c r="R23" s="3">
         <v>800</v>
       </c>
-      <c r="S23" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -2622,11 +2555,11 @@
       <c r="H24">
         <v>267.11094359397077</v>
       </c>
-      <c r="I24">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
       </c>
       <c r="K24" s="3">
         <v>0</v>
@@ -2635,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N24" s="3">
         <v>800</v>
@@ -2652,11 +2585,8 @@
       <c r="R24" s="3">
         <v>800</v>
       </c>
-      <c r="S24" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2681,11 +2611,11 @@
       <c r="H25">
         <v>236.32090194917032</v>
       </c>
-      <c r="I25">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J25" s="2">
-        <v>1</v>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
       </c>
       <c r="K25" s="3">
         <v>0</v>
@@ -2694,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N25" s="3">
         <v>800</v>
@@ -2711,11 +2641,8 @@
       <c r="R25" s="3">
         <v>800</v>
       </c>
-      <c r="S25" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2740,11 +2667,11 @@
       <c r="H26">
         <v>268.84800000000001</v>
       </c>
-      <c r="I26">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J26" s="2">
-        <v>1</v>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
       </c>
       <c r="K26" s="3">
         <v>0</v>
@@ -2753,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N26" s="3">
         <v>800</v>
@@ -2770,11 +2697,8 @@
       <c r="R26" s="3">
         <v>800</v>
       </c>
-      <c r="S26" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2799,11 +2723,11 @@
       <c r="H27">
         <v>333.21600000000001</v>
       </c>
-      <c r="I27">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1</v>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
       </c>
       <c r="K27" s="3">
         <v>0</v>
@@ -2812,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N27" s="3">
         <v>800</v>
@@ -2829,11 +2753,8 @@
       <c r="R27" s="3">
         <v>800</v>
       </c>
-      <c r="S27" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2858,11 +2779,11 @@
       <c r="H28">
         <v>304.457671</v>
       </c>
-      <c r="I28">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J28" s="2">
-        <v>1</v>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
       </c>
       <c r="K28" s="3">
         <v>0</v>
@@ -2871,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N28" s="3">
         <v>800</v>
@@ -2888,11 +2809,8 @@
       <c r="R28" s="3">
         <v>800</v>
       </c>
-      <c r="S28" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2917,11 +2835,11 @@
       <c r="H29">
         <v>272.8332297733578</v>
       </c>
-      <c r="I29">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J29" s="2">
-        <v>1</v>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
       </c>
       <c r="K29" s="3">
         <v>0</v>
@@ -2930,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N29" s="3">
         <v>800</v>
@@ -2947,11 +2865,8 @@
       <c r="R29" s="3">
         <v>800</v>
       </c>
-      <c r="S29" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2976,11 +2891,11 @@
       <c r="H30">
         <v>279.06071328318535</v>
       </c>
-      <c r="I30">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
       </c>
       <c r="K30" s="3">
         <v>0</v>
@@ -2989,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N30" s="3">
         <v>800</v>
@@ -3006,11 +2921,8 @@
       <c r="R30" s="3">
         <v>800</v>
       </c>
-      <c r="S30" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -3035,11 +2947,11 @@
       <c r="H31">
         <v>318.39373953550853</v>
       </c>
-      <c r="I31">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
       </c>
       <c r="K31" s="3">
         <v>0</v>
@@ -3048,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N31" s="3">
         <v>800</v>
@@ -3065,11 +2977,8 @@
       <c r="R31" s="3">
         <v>800</v>
       </c>
-      <c r="S31" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -3094,11 +3003,11 @@
       <c r="H32">
         <v>313.6028283502921</v>
       </c>
-      <c r="I32">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1</v>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
       </c>
       <c r="K32" s="3">
         <v>0</v>
@@ -3107,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N32" s="3">
         <v>800</v>
@@ -3124,11 +3033,8 @@
       <c r="R32" s="3">
         <v>800</v>
       </c>
-      <c r="S32" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -3153,11 +3059,11 @@
       <c r="H33">
         <v>303.20310115527809</v>
       </c>
-      <c r="I33">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J33" s="2">
-        <v>1</v>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
       </c>
       <c r="K33" s="3">
         <v>0</v>
@@ -3166,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N33" s="3">
         <v>800</v>
@@ -3183,11 +3089,8 @@
       <c r="R33" s="3">
         <v>800</v>
       </c>
-      <c r="S33" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -3212,11 +3115,11 @@
       <c r="H34">
         <v>309.72708726376976</v>
       </c>
-      <c r="I34">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J34" s="2">
-        <v>1</v>
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
       </c>
       <c r="K34" s="3">
         <v>0</v>
@@ -3225,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N34" s="3">
         <v>800</v>
@@ -3242,11 +3145,8 @@
       <c r="R34" s="3">
         <v>800</v>
       </c>
-      <c r="S34" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -3271,11 +3171,11 @@
       <c r="H35">
         <v>278.46519876343689</v>
       </c>
-      <c r="I35">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J35" s="2">
-        <v>1</v>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
       </c>
       <c r="K35" s="3">
         <v>0</v>
@@ -3284,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N35" s="3">
         <v>800</v>
@@ -3301,11 +3201,8 @@
       <c r="R35" s="3">
         <v>800</v>
       </c>
-      <c r="S35" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -3330,11 +3227,11 @@
       <c r="H36">
         <v>292.06251901012189</v>
       </c>
-      <c r="I36">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J36" s="2">
-        <v>1</v>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
       </c>
       <c r="K36" s="3">
         <v>0</v>
@@ -3343,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N36" s="3">
         <v>800</v>
@@ -3360,11 +3257,8 @@
       <c r="R36" s="3">
         <v>800</v>
       </c>
-      <c r="S36" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3389,11 +3283,11 @@
       <c r="H37">
         <v>310.03998424384974</v>
       </c>
-      <c r="I37">
-        <v>0.32480000000000003</v>
-      </c>
-      <c r="J37" s="2">
-        <v>1</v>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
@@ -3402,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N37" s="3">
         <v>800</v>
@@ -3419,11 +3313,8 @@
       <c r="R37" s="3">
         <v>800</v>
       </c>
-      <c r="S37" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -3448,11 +3339,11 @@
       <c r="H38">
         <v>136.78</v>
       </c>
-      <c r="I38">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J38" s="2">
-        <v>1</v>
+      <c r="I38" s="2">
+        <v>1</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
       </c>
       <c r="K38" s="3">
         <v>0</v>
@@ -3461,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N38" s="3">
         <v>800</v>
@@ -3478,11 +3369,8 @@
       <c r="R38" s="3">
         <v>800</v>
       </c>
-      <c r="S38" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -3507,11 +3395,11 @@
       <c r="H39">
         <v>260.26</v>
       </c>
-      <c r="I39">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J39" s="2">
-        <v>1</v>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
       </c>
       <c r="K39" s="3">
         <v>0</v>
@@ -3520,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N39" s="3">
         <v>800</v>
@@ -3537,11 +3425,8 @@
       <c r="R39" s="3">
         <v>800</v>
       </c>
-      <c r="S39" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -3566,11 +3451,11 @@
       <c r="H40">
         <v>162.097083</v>
       </c>
-      <c r="I40">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J40" s="2">
-        <v>1</v>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0</v>
       </c>
       <c r="K40" s="3">
         <v>0</v>
@@ -3579,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N40" s="3">
         <v>800</v>
@@ -3596,11 +3481,8 @@
       <c r="R40" s="3">
         <v>800</v>
       </c>
-      <c r="S40" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -3625,11 +3507,11 @@
       <c r="H41">
         <v>441.96</v>
       </c>
-      <c r="I41">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J41" s="2">
-        <v>1</v>
+      <c r="I41" s="2">
+        <v>1</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
@@ -3638,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N41" s="3">
         <v>800</v>
@@ -3655,11 +3537,8 @@
       <c r="R41" s="3">
         <v>800</v>
       </c>
-      <c r="S41" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -3684,11 +3563,11 @@
       <c r="H42">
         <v>437.16800000000001</v>
       </c>
-      <c r="I42">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J42" s="2">
-        <v>1</v>
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
       </c>
       <c r="K42" s="3">
         <v>0</v>
@@ -3697,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N42" s="3">
         <v>800</v>
@@ -3714,11 +3593,8 @@
       <c r="R42" s="3">
         <v>800</v>
       </c>
-      <c r="S42" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -3743,11 +3619,11 @@
       <c r="H43">
         <v>455.52376000000004</v>
       </c>
-      <c r="I43">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J43" s="2">
-        <v>1</v>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
       </c>
       <c r="K43" s="3">
         <v>0</v>
@@ -3756,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N43" s="3">
         <v>800</v>
@@ -3773,11 +3649,8 @@
       <c r="R43" s="3">
         <v>800</v>
       </c>
-      <c r="S43" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -3802,11 +3675,11 @@
       <c r="H44">
         <v>438.38656000000003</v>
       </c>
-      <c r="I44">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J44" s="2">
-        <v>1</v>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
       </c>
       <c r="K44" s="3">
         <v>0</v>
@@ -3815,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N44" s="3">
         <v>800</v>
@@ -3832,11 +3705,8 @@
       <c r="R44" s="3">
         <v>800</v>
       </c>
-      <c r="S44" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -3861,11 +3731,11 @@
       <c r="H45">
         <v>439.709248</v>
       </c>
-      <c r="I45">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J45" s="2">
-        <v>1</v>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
       </c>
       <c r="K45" s="3">
         <v>0</v>
@@ -3874,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N45" s="3">
         <v>800</v>
@@ -3891,11 +3761,8 @@
       <c r="R45" s="3">
         <v>800</v>
       </c>
-      <c r="S45" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -3920,11 +3787,11 @@
       <c r="H46">
         <v>437.88479999999998</v>
       </c>
-      <c r="I46">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J46" s="2">
-        <v>1</v>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
       </c>
       <c r="K46" s="3">
         <v>0</v>
@@ -3933,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N46" s="3">
         <v>800</v>
@@ -3950,11 +3817,8 @@
       <c r="R46" s="3">
         <v>800</v>
       </c>
-      <c r="S46" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -3979,11 +3843,11 @@
       <c r="H47">
         <v>176.56413126832402</v>
       </c>
-      <c r="I47">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J47" s="2">
-        <v>1</v>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
       </c>
       <c r="K47" s="3">
         <v>0</v>
@@ -3992,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N47" s="3">
         <v>800</v>
@@ -4009,11 +3873,8 @@
       <c r="R47" s="3">
         <v>800</v>
       </c>
-      <c r="S47" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -4038,11 +3899,11 @@
       <c r="H48">
         <v>175.87293261359494</v>
       </c>
-      <c r="I48">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J48" s="2">
-        <v>1</v>
+      <c r="I48" s="2">
+        <v>1</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0</v>
       </c>
       <c r="K48" s="3">
         <v>0</v>
@@ -4051,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N48" s="3">
         <v>800</v>
@@ -4068,11 +3929,8 @@
       <c r="R48" s="3">
         <v>800</v>
       </c>
-      <c r="S48" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -4097,11 +3955,11 @@
       <c r="H49">
         <v>180.96022542822678</v>
       </c>
-      <c r="I49">
-        <v>0.30080000000000001</v>
-      </c>
-      <c r="J49" s="2">
-        <v>1</v>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0</v>
       </c>
       <c r="K49" s="3">
         <v>0</v>
@@ -4110,7 +3968,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N49" s="3">
         <v>800</v>
@@ -4127,11 +3985,8 @@
       <c r="R49" s="3">
         <v>800</v>
       </c>
-      <c r="S49" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -4156,11 +4011,11 @@
       <c r="H50">
         <v>380.97199999999998</v>
       </c>
-      <c r="I50">
-        <v>0.2359</v>
-      </c>
-      <c r="J50" s="2">
-        <v>1</v>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
       </c>
       <c r="K50" s="3">
         <v>0</v>
@@ -4169,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N50" s="3">
         <v>800</v>
@@ -4186,11 +4041,8 @@
       <c r="R50" s="3">
         <v>800</v>
       </c>
-      <c r="S50" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -4215,11 +4067,11 @@
       <c r="H51">
         <v>387.32</v>
       </c>
-      <c r="I51">
-        <v>0.2359</v>
-      </c>
-      <c r="J51" s="2">
-        <v>1</v>
+      <c r="I51" s="2">
+        <v>1</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0</v>
       </c>
       <c r="K51" s="3">
         <v>0</v>
@@ -4228,7 +4080,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N51" s="3">
         <v>800</v>
@@ -4245,11 +4097,8 @@
       <c r="R51" s="3">
         <v>800</v>
       </c>
-      <c r="S51" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
@@ -4274,11 +4123,11 @@
       <c r="H52">
         <v>315.05490600000002</v>
       </c>
-      <c r="I52">
-        <v>0.2359</v>
-      </c>
-      <c r="J52" s="2">
-        <v>1</v>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
       </c>
       <c r="K52" s="3">
         <v>0</v>
@@ -4287,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N52" s="3">
         <v>800</v>
@@ -4304,11 +4153,8 @@
       <c r="R52" s="3">
         <v>800</v>
       </c>
-      <c r="S52" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -4333,11 +4179,11 @@
       <c r="H53">
         <v>374.61471999999998</v>
       </c>
-      <c r="I53">
-        <v>0.2359</v>
-      </c>
-      <c r="J53" s="2">
-        <v>1</v>
+      <c r="I53" s="2">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0</v>
       </c>
       <c r="K53" s="3">
         <v>0</v>
@@ -4346,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N53" s="3">
         <v>800</v>
@@ -4363,11 +4209,8 @@
       <c r="R53" s="3">
         <v>800</v>
       </c>
-      <c r="S53" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
@@ -4392,11 +4235,11 @@
       <c r="H54">
         <v>497.18183199999993</v>
       </c>
-      <c r="I54">
-        <v>0.2359</v>
-      </c>
-      <c r="J54" s="2">
-        <v>1</v>
+      <c r="I54" s="2">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
       </c>
       <c r="K54" s="3">
         <v>0</v>
@@ -4405,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N54" s="3">
         <v>800</v>
@@ -4422,11 +4265,8 @@
       <c r="R54" s="3">
         <v>800</v>
       </c>
-      <c r="S54" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -4451,11 +4291,11 @@
       <c r="H55">
         <v>570.50842799999998</v>
       </c>
-      <c r="I55">
-        <v>0.2359</v>
-      </c>
-      <c r="J55" s="2">
-        <v>1</v>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
       </c>
       <c r="K55" s="3">
         <v>0</v>
@@ -4464,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N55" s="3">
         <v>800</v>
@@ -4481,11 +4321,8 @@
       <c r="R55" s="3">
         <v>800</v>
       </c>
-      <c r="S55" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
@@ -4510,11 +4347,11 @@
       <c r="H56">
         <v>407.3501</v>
       </c>
-      <c r="I56">
-        <v>0.2359</v>
-      </c>
-      <c r="J56" s="2">
-        <v>1</v>
+      <c r="I56" s="2">
+        <v>1</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0</v>
       </c>
       <c r="K56" s="3">
         <v>0</v>
@@ -4523,7 +4360,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N56" s="3">
         <v>800</v>
@@ -4540,11 +4377,8 @@
       <c r="R56" s="3">
         <v>800</v>
       </c>
-      <c r="S56" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -4569,11 +4403,11 @@
       <c r="H57">
         <v>426.08867900000001</v>
       </c>
-      <c r="I57">
-        <v>0.2359</v>
-      </c>
-      <c r="J57" s="2">
-        <v>1</v>
+      <c r="I57" s="2">
+        <v>1</v>
+      </c>
+      <c r="J57" s="3">
+        <v>0</v>
       </c>
       <c r="K57" s="3">
         <v>0</v>
@@ -4582,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N57" s="3">
         <v>800</v>
@@ -4599,11 +4433,8 @@
       <c r="R57" s="3">
         <v>800</v>
       </c>
-      <c r="S57" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -4628,11 +4459,11 @@
       <c r="H58">
         <v>406.63618000000002</v>
       </c>
-      <c r="I58">
-        <v>0.2359</v>
-      </c>
-      <c r="J58" s="2">
-        <v>1</v>
+      <c r="I58" s="2">
+        <v>1</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0</v>
       </c>
       <c r="K58" s="3">
         <v>0</v>
@@ -4641,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N58" s="3">
         <v>800</v>
@@ -4658,11 +4489,8 @@
       <c r="R58" s="3">
         <v>800</v>
       </c>
-      <c r="S58" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -4687,11 +4515,11 @@
       <c r="H59">
         <v>399.50447606837997</v>
       </c>
-      <c r="I59">
-        <v>0.2359</v>
-      </c>
-      <c r="J59" s="2">
-        <v>1</v>
+      <c r="I59" s="2">
+        <v>1</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
       </c>
       <c r="K59" s="3">
         <v>0</v>
@@ -4700,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N59" s="3">
         <v>800</v>
@@ -4717,11 +4545,8 @@
       <c r="R59" s="3">
         <v>800</v>
       </c>
-      <c r="S59" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
@@ -4746,11 +4571,11 @@
       <c r="H60">
         <v>326.82910014606676</v>
       </c>
-      <c r="I60">
-        <v>0.2359</v>
-      </c>
-      <c r="J60" s="2">
-        <v>1</v>
+      <c r="I60" s="2">
+        <v>1</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0</v>
       </c>
       <c r="K60" s="3">
         <v>0</v>
@@ -4759,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N60" s="3">
         <v>800</v>
@@ -4776,11 +4601,8 @@
       <c r="R60" s="3">
         <v>800</v>
       </c>
-      <c r="S60" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -4805,11 +4627,11 @@
       <c r="H61">
         <v>312.6476424297922</v>
       </c>
-      <c r="I61">
-        <v>0.2359</v>
-      </c>
-      <c r="J61" s="2">
-        <v>1</v>
+      <c r="I61" s="2">
+        <v>1</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0</v>
       </c>
       <c r="K61" s="3">
         <v>0</v>
@@ -4818,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N61" s="3">
         <v>800</v>
@@ -4835,11 +4657,8 @@
       <c r="R61" s="3">
         <v>800</v>
       </c>
-      <c r="S61" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -4864,11 +4683,11 @@
       <c r="H62">
         <v>66.959999999999994</v>
       </c>
-      <c r="I62">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J62" s="2">
-        <v>1</v>
+      <c r="I62" s="2">
+        <v>1</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0</v>
       </c>
       <c r="K62" s="3">
         <v>0</v>
@@ -4877,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N62" s="3">
         <v>800</v>
@@ -4894,11 +4713,8 @@
       <c r="R62" s="3">
         <v>800</v>
       </c>
-      <c r="S62" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -4923,11 +4739,11 @@
       <c r="H63">
         <v>40.08</v>
       </c>
-      <c r="I63">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J63" s="2">
-        <v>1</v>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0</v>
       </c>
       <c r="K63" s="3">
         <v>0</v>
@@ -4936,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N63" s="3">
         <v>800</v>
@@ -4953,11 +4769,8 @@
       <c r="R63" s="3">
         <v>800</v>
       </c>
-      <c r="S63" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -4982,11 +4795,11 @@
       <c r="H64">
         <v>80.170997</v>
       </c>
-      <c r="I64">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J64" s="2">
-        <v>1</v>
+      <c r="I64" s="2">
+        <v>1</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0</v>
       </c>
       <c r="K64" s="3">
         <v>0</v>
@@ -4995,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N64" s="3">
         <v>800</v>
@@ -5012,11 +4825,8 @@
       <c r="R64" s="3">
         <v>800</v>
       </c>
-      <c r="S64" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -5041,11 +4851,11 @@
       <c r="H65">
         <v>75.114166666666662</v>
       </c>
-      <c r="I65">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J65" s="2">
-        <v>1</v>
+      <c r="I65" s="2">
+        <v>1</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
       </c>
       <c r="K65" s="3">
         <v>0</v>
@@ -5054,7 +4864,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N65" s="3">
         <v>800</v>
@@ -5071,11 +4881,8 @@
       <c r="R65" s="3">
         <v>800</v>
       </c>
-      <c r="S65" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -5100,11 +4907,11 @@
       <c r="H66">
         <v>75.117916666666673</v>
       </c>
-      <c r="I66">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J66" s="2">
-        <v>1</v>
+      <c r="I66" s="2">
+        <v>1</v>
+      </c>
+      <c r="J66" s="3">
+        <v>0</v>
       </c>
       <c r="K66" s="3">
         <v>0</v>
@@ -5113,7 +4920,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N66" s="3">
         <v>800</v>
@@ -5130,11 +4937,8 @@
       <c r="R66" s="3">
         <v>800</v>
       </c>
-      <c r="S66" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -5159,11 +4963,11 @@
       <c r="H67">
         <v>45.119166666666665</v>
       </c>
-      <c r="I67">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J67" s="2">
-        <v>1</v>
+      <c r="I67" s="2">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
       </c>
       <c r="K67" s="3">
         <v>0</v>
@@ -5172,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N67" s="3">
         <v>800</v>
@@ -5189,11 +4993,8 @@
       <c r="R67" s="3">
         <v>800</v>
       </c>
-      <c r="S67" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -5218,11 +5019,11 @@
       <c r="H68">
         <v>45.100416666666668</v>
       </c>
-      <c r="I68">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J68" s="2">
-        <v>1</v>
+      <c r="I68" s="2">
+        <v>1</v>
+      </c>
+      <c r="J68" s="3">
+        <v>0</v>
       </c>
       <c r="K68" s="3">
         <v>0</v>
@@ -5231,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N68" s="3">
         <v>800</v>
@@ -5248,11 +5049,8 @@
       <c r="R68" s="3">
         <v>800</v>
       </c>
-      <c r="S68" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -5277,11 +5075,11 @@
       <c r="H69">
         <v>45.100833333333334</v>
       </c>
-      <c r="I69">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J69" s="2">
-        <v>1</v>
+      <c r="I69" s="2">
+        <v>1</v>
+      </c>
+      <c r="J69" s="3">
+        <v>0</v>
       </c>
       <c r="K69" s="3">
         <v>0</v>
@@ -5290,7 +5088,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N69" s="3">
         <v>800</v>
@@ -5307,11 +5105,8 @@
       <c r="R69" s="3">
         <v>800</v>
       </c>
-      <c r="S69" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -5336,11 +5131,11 @@
       <c r="H70">
         <v>45.091666666666669</v>
       </c>
-      <c r="I70">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J70" s="2">
-        <v>1</v>
+      <c r="I70" s="2">
+        <v>1</v>
+      </c>
+      <c r="J70" s="3">
+        <v>0</v>
       </c>
       <c r="K70" s="3">
         <v>0</v>
@@ -5349,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N70" s="3">
         <v>800</v>
@@ -5366,11 +5161,8 @@
       <c r="R70" s="3">
         <v>800</v>
       </c>
-      <c r="S70" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -5395,11 +5187,11 @@
       <c r="H71">
         <v>393.36201270243765</v>
       </c>
-      <c r="I71">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J71" s="2">
-        <v>1</v>
+      <c r="I71" s="2">
+        <v>1</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0</v>
       </c>
       <c r="K71" s="3">
         <v>0</v>
@@ -5408,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N71" s="3">
         <v>800</v>
@@ -5425,11 +5217,8 @@
       <c r="R71" s="3">
         <v>800</v>
       </c>
-      <c r="S71" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -5454,11 +5243,11 @@
       <c r="H72">
         <v>358.04153088711774</v>
       </c>
-      <c r="I72">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J72" s="2">
-        <v>1</v>
+      <c r="I72" s="2">
+        <v>1</v>
+      </c>
+      <c r="J72" s="3">
+        <v>0</v>
       </c>
       <c r="K72" s="3">
         <v>0</v>
@@ -5467,7 +5256,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N72" s="3">
         <v>800</v>
@@ -5484,11 +5273,8 @@
       <c r="R72" s="3">
         <v>800</v>
       </c>
-      <c r="S72" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -5513,11 +5299,11 @@
       <c r="H73">
         <v>297.00256773827164</v>
       </c>
-      <c r="I73">
-        <v>0.24869999999999998</v>
-      </c>
-      <c r="J73" s="2">
-        <v>1</v>
+      <c r="I73" s="2">
+        <v>1</v>
+      </c>
+      <c r="J73" s="3">
+        <v>0</v>
       </c>
       <c r="K73" s="3">
         <v>0</v>
@@ -5526,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N73" s="3">
         <v>800</v>
@@ -5543,11 +5329,8 @@
       <c r="R73" s="3">
         <v>800</v>
       </c>
-      <c r="S73" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>6</v>
       </c>
@@ -5572,11 +5355,11 @@
       <c r="H74">
         <v>172.16</v>
       </c>
-      <c r="I74">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J74" s="2">
-        <v>1</v>
+      <c r="I74" s="2">
+        <v>1</v>
+      </c>
+      <c r="J74" s="3">
+        <v>0</v>
       </c>
       <c r="K74" s="3">
         <v>0</v>
@@ -5585,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N74" s="3">
         <v>800</v>
@@ -5602,11 +5385,8 @@
       <c r="R74" s="3">
         <v>800</v>
       </c>
-      <c r="S74" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -5631,11 +5411,11 @@
       <c r="H75">
         <v>351.84</v>
       </c>
-      <c r="I75">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J75" s="2">
-        <v>1</v>
+      <c r="I75" s="2">
+        <v>1</v>
+      </c>
+      <c r="J75" s="3">
+        <v>0</v>
       </c>
       <c r="K75" s="3">
         <v>0</v>
@@ -5644,7 +5424,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N75" s="3">
         <v>800</v>
@@ -5661,11 +5441,8 @@
       <c r="R75" s="3">
         <v>800</v>
       </c>
-      <c r="S75" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -5690,11 +5467,11 @@
       <c r="H76">
         <v>322.381328</v>
       </c>
-      <c r="I76">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J76" s="2">
-        <v>1</v>
+      <c r="I76" s="2">
+        <v>1</v>
+      </c>
+      <c r="J76" s="3">
+        <v>0</v>
       </c>
       <c r="K76" s="3">
         <v>0</v>
@@ -5703,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="M76" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N76" s="3">
         <v>800</v>
@@ -5720,11 +5497,8 @@
       <c r="R76" s="3">
         <v>800</v>
       </c>
-      <c r="S76" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
@@ -5749,11 +5523,11 @@
       <c r="H77">
         <v>226.6507635443968</v>
       </c>
-      <c r="I77">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J77" s="2">
-        <v>1</v>
+      <c r="I77" s="2">
+        <v>1</v>
+      </c>
+      <c r="J77" s="3">
+        <v>0</v>
       </c>
       <c r="K77" s="3">
         <v>0</v>
@@ -5762,7 +5536,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N77" s="3">
         <v>800</v>
@@ -5779,11 +5553,8 @@
       <c r="R77" s="3">
         <v>800</v>
       </c>
-      <c r="S77" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -5808,11 +5579,11 @@
       <c r="H78">
         <v>225.98216460990884</v>
       </c>
-      <c r="I78">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J78" s="2">
-        <v>1</v>
+      <c r="I78" s="2">
+        <v>1</v>
+      </c>
+      <c r="J78" s="3">
+        <v>0</v>
       </c>
       <c r="K78" s="3">
         <v>0</v>
@@ -5821,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N78" s="3">
         <v>800</v>
@@ -5838,11 +5609,8 @@
       <c r="R78" s="3">
         <v>800</v>
       </c>
-      <c r="S78" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -5867,11 +5635,11 @@
       <c r="H79">
         <v>267.529010551385</v>
       </c>
-      <c r="I79">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J79" s="2">
-        <v>1</v>
+      <c r="I79" s="2">
+        <v>1</v>
+      </c>
+      <c r="J79" s="3">
+        <v>0</v>
       </c>
       <c r="K79" s="3">
         <v>0</v>
@@ -5880,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N79" s="3">
         <v>800</v>
@@ -5897,11 +5665,8 @@
       <c r="R79" s="3">
         <v>800</v>
       </c>
-      <c r="S79" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>6</v>
       </c>
@@ -5926,11 +5691,11 @@
       <c r="H80">
         <v>250.26577200718117</v>
       </c>
-      <c r="I80">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J80" s="2">
-        <v>1</v>
+      <c r="I80" s="2">
+        <v>1</v>
+      </c>
+      <c r="J80" s="3">
+        <v>0</v>
       </c>
       <c r="K80" s="3">
         <v>0</v>
@@ -5939,7 +5704,7 @@
         <v>0</v>
       </c>
       <c r="M80" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N80" s="3">
         <v>800</v>
@@ -5956,11 +5721,8 @@
       <c r="R80" s="3">
         <v>800</v>
       </c>
-      <c r="S80" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>6</v>
       </c>
@@ -5985,11 +5747,11 @@
       <c r="H81">
         <v>261.04566421503432</v>
       </c>
-      <c r="I81">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J81" s="2">
-        <v>1</v>
+      <c r="I81" s="2">
+        <v>1</v>
+      </c>
+      <c r="J81" s="3">
+        <v>0</v>
       </c>
       <c r="K81" s="3">
         <v>0</v>
@@ -5998,7 +5760,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N81" s="3">
         <v>800</v>
@@ -6015,11 +5777,8 @@
       <c r="R81" s="3">
         <v>800</v>
       </c>
-      <c r="S81" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -6044,11 +5803,11 @@
       <c r="H82">
         <v>258.21249576382229</v>
       </c>
-      <c r="I82">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J82" s="2">
-        <v>1</v>
+      <c r="I82" s="2">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3">
+        <v>0</v>
       </c>
       <c r="K82" s="3">
         <v>0</v>
@@ -6057,7 +5816,7 @@
         <v>0</v>
       </c>
       <c r="M82" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N82" s="3">
         <v>800</v>
@@ -6074,11 +5833,8 @@
       <c r="R82" s="3">
         <v>800</v>
       </c>
-      <c r="S82" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>6</v>
       </c>
@@ -6103,11 +5859,11 @@
       <c r="H83">
         <v>286.31673768860531</v>
       </c>
-      <c r="I83">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J83" s="2">
-        <v>1</v>
+      <c r="I83" s="2">
+        <v>1</v>
+      </c>
+      <c r="J83" s="3">
+        <v>0</v>
       </c>
       <c r="K83" s="3">
         <v>0</v>
@@ -6116,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N83" s="3">
         <v>800</v>
@@ -6133,11 +5889,8 @@
       <c r="R83" s="3">
         <v>800</v>
       </c>
-      <c r="S83" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -6162,11 +5915,11 @@
       <c r="H84">
         <v>293.95087793952791</v>
       </c>
-      <c r="I84">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J84" s="2">
-        <v>1</v>
+      <c r="I84" s="2">
+        <v>1</v>
+      </c>
+      <c r="J84" s="3">
+        <v>0</v>
       </c>
       <c r="K84" s="3">
         <v>0</v>
@@ -6175,7 +5928,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N84" s="3">
         <v>800</v>
@@ -6192,11 +5945,8 @@
       <c r="R84" s="3">
         <v>800</v>
       </c>
-      <c r="S84" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
@@ -6221,11 +5971,11 @@
       <c r="H85">
         <v>312.65864104690036</v>
       </c>
-      <c r="I85">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J85" s="2">
-        <v>1</v>
+      <c r="I85" s="2">
+        <v>1</v>
+      </c>
+      <c r="J85" s="3">
+        <v>0</v>
       </c>
       <c r="K85" s="3">
         <v>0</v>
@@ -6234,7 +5984,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N85" s="3">
         <v>800</v>
@@ -6251,11 +6001,8 @@
       <c r="R85" s="3">
         <v>800</v>
       </c>
-      <c r="S85" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
@@ -6280,11 +6027,11 @@
       <c r="H86" s="4">
         <v>15888</v>
       </c>
-      <c r="I86">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J86" s="2">
-        <v>1</v>
+      <c r="I86" s="2">
+        <v>1</v>
+      </c>
+      <c r="J86" s="3">
+        <v>0</v>
       </c>
       <c r="K86" s="3">
         <v>0</v>
@@ -6293,7 +6040,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N86" s="3">
         <v>800</v>
@@ -6310,11 +6057,8 @@
       <c r="R86" s="3">
         <v>800</v>
       </c>
-      <c r="S86" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
@@ -6339,11 +6083,11 @@
       <c r="H87">
         <v>216</v>
       </c>
-      <c r="I87">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J87" s="2">
-        <v>1</v>
+      <c r="I87" s="2">
+        <v>1</v>
+      </c>
+      <c r="J87" s="3">
+        <v>0</v>
       </c>
       <c r="K87" s="3">
         <v>0</v>
@@ -6352,7 +6096,7 @@
         <v>0</v>
       </c>
       <c r="M87" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N87" s="3">
         <v>800</v>
@@ -6369,11 +6113,8 @@
       <c r="R87" s="3">
         <v>800</v>
       </c>
-      <c r="S87" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -6398,11 +6139,11 @@
       <c r="H88">
         <v>191.73523</v>
       </c>
-      <c r="I88">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J88" s="2">
-        <v>1</v>
+      <c r="I88" s="2">
+        <v>1</v>
+      </c>
+      <c r="J88" s="3">
+        <v>0</v>
       </c>
       <c r="K88" s="3">
         <v>0</v>
@@ -6411,7 +6152,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N88" s="3">
         <v>800</v>
@@ -6428,11 +6169,8 @@
       <c r="R88" s="3">
         <v>800</v>
       </c>
-      <c r="S88" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>7</v>
       </c>
@@ -6457,11 +6195,11 @@
       <c r="H89">
         <v>183.86997171418238</v>
       </c>
-      <c r="I89">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J89" s="2">
-        <v>1</v>
+      <c r="I89" s="2">
+        <v>1</v>
+      </c>
+      <c r="J89" s="3">
+        <v>0</v>
       </c>
       <c r="K89" s="3">
         <v>0</v>
@@ -6470,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="M89" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N89" s="3">
         <v>800</v>
@@ -6487,11 +6225,8 @@
       <c r="R89" s="3">
         <v>800</v>
       </c>
-      <c r="S89" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>7</v>
       </c>
@@ -6516,11 +6251,11 @@
       <c r="H90">
         <v>182.15497376866915</v>
       </c>
-      <c r="I90">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J90" s="2">
-        <v>1</v>
+      <c r="I90" s="2">
+        <v>1</v>
+      </c>
+      <c r="J90" s="3">
+        <v>0</v>
       </c>
       <c r="K90" s="3">
         <v>0</v>
@@ -6529,7 +6264,7 @@
         <v>0</v>
       </c>
       <c r="M90" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N90" s="3">
         <v>800</v>
@@ -6546,11 +6281,8 @@
       <c r="R90" s="3">
         <v>800</v>
       </c>
-      <c r="S90" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
@@ -6575,11 +6307,11 @@
       <c r="H91">
         <v>203.73091101602503</v>
       </c>
-      <c r="I91">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J91" s="2">
-        <v>1</v>
+      <c r="I91" s="2">
+        <v>1</v>
+      </c>
+      <c r="J91" s="3">
+        <v>0</v>
       </c>
       <c r="K91" s="3">
         <v>0</v>
@@ -6588,7 +6320,7 @@
         <v>0</v>
       </c>
       <c r="M91" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N91" s="3">
         <v>800</v>
@@ -6605,11 +6337,8 @@
       <c r="R91" s="3">
         <v>800</v>
       </c>
-      <c r="S91" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
@@ -6634,11 +6363,11 @@
       <c r="H92">
         <v>188.61925192356389</v>
       </c>
-      <c r="I92">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J92" s="2">
-        <v>1</v>
+      <c r="I92" s="2">
+        <v>1</v>
+      </c>
+      <c r="J92" s="3">
+        <v>0</v>
       </c>
       <c r="K92" s="3">
         <v>0</v>
@@ -6647,7 +6376,7 @@
         <v>0</v>
       </c>
       <c r="M92" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N92" s="3">
         <v>800</v>
@@ -6664,11 +6393,8 @@
       <c r="R92" s="3">
         <v>800</v>
       </c>
-      <c r="S92" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
@@ -6693,11 +6419,11 @@
       <c r="H93">
         <v>174.6351374791916</v>
       </c>
-      <c r="I93">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J93" s="2">
-        <v>1</v>
+      <c r="I93" s="2">
+        <v>1</v>
+      </c>
+      <c r="J93" s="3">
+        <v>0</v>
       </c>
       <c r="K93" s="3">
         <v>0</v>
@@ -6706,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N93" s="3">
         <v>800</v>
@@ -6723,11 +6449,8 @@
       <c r="R93" s="3">
         <v>800</v>
       </c>
-      <c r="S93" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
@@ -6752,11 +6475,11 @@
       <c r="H94">
         <v>182.50702688818998</v>
       </c>
-      <c r="I94">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J94" s="2">
-        <v>1</v>
+      <c r="I94" s="2">
+        <v>1</v>
+      </c>
+      <c r="J94" s="3">
+        <v>0</v>
       </c>
       <c r="K94" s="3">
         <v>0</v>
@@ -6765,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="M94" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N94" s="3">
         <v>800</v>
@@ -6782,11 +6505,8 @@
       <c r="R94" s="3">
         <v>800</v>
       </c>
-      <c r="S94" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>7</v>
       </c>
@@ -6811,11 +6531,11 @@
       <c r="H95">
         <v>161.39232668881274</v>
       </c>
-      <c r="I95">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J95" s="2">
-        <v>1</v>
+      <c r="I95" s="2">
+        <v>1</v>
+      </c>
+      <c r="J95" s="3">
+        <v>0</v>
       </c>
       <c r="K95" s="3">
         <v>0</v>
@@ -6824,7 +6544,7 @@
         <v>0</v>
       </c>
       <c r="M95" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N95" s="3">
         <v>800</v>
@@ -6841,11 +6561,8 @@
       <c r="R95" s="3">
         <v>800</v>
       </c>
-      <c r="S95" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
@@ -6870,11 +6587,11 @@
       <c r="H96">
         <v>179.85032209786073</v>
       </c>
-      <c r="I96">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J96" s="2">
-        <v>1</v>
+      <c r="I96" s="2">
+        <v>1</v>
+      </c>
+      <c r="J96" s="3">
+        <v>0</v>
       </c>
       <c r="K96" s="3">
         <v>0</v>
@@ -6883,7 +6600,7 @@
         <v>0</v>
       </c>
       <c r="M96" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N96" s="3">
         <v>800</v>
@@ -6900,11 +6617,8 @@
       <c r="R96" s="3">
         <v>800</v>
       </c>
-      <c r="S96" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>7</v>
       </c>
@@ -6929,11 +6643,11 @@
       <c r="H97">
         <v>182.10758456314562</v>
       </c>
-      <c r="I97">
-        <v>0.29239999999999999</v>
-      </c>
-      <c r="J97" s="2">
-        <v>1</v>
+      <c r="I97" s="2">
+        <v>1</v>
+      </c>
+      <c r="J97" s="3">
+        <v>0</v>
       </c>
       <c r="K97" s="3">
         <v>0</v>
@@ -6942,7 +6656,7 @@
         <v>0</v>
       </c>
       <c r="M97" s="3">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N97" s="3">
         <v>800</v>
@@ -6959,12 +6673,9 @@
       <c r="R97" s="3">
         <v>800</v>
       </c>
-      <c r="S97" s="3">
-        <v>800</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -6987,36 +6698,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -7045,7 +6756,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6">
         <v>12</v>
@@ -7074,7 +6785,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6">
         <v>15</v>
@@ -7103,7 +6814,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6">
         <v>45</v>
@@ -7132,7 +6843,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6">
         <v>50</v>
@@ -7161,7 +6872,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6">
         <v>30</v>
@@ -7190,7 +6901,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
         <v>60</v>
@@ -7219,7 +6930,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6">
         <v>10</v>
@@ -7258,10 +6969,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M25"/>
+    <sheetView topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7278,48 +6989,54 @@
     <col min="11" max="11" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7359,8 +7076,14 @@
       <c r="M2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7400,8 +7123,14 @@
       <c r="M3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7441,8 +7170,14 @@
       <c r="M4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7482,8 +7217,14 @@
       <c r="M5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -7523,8 +7264,14 @@
       <c r="M6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -7564,8 +7311,14 @@
       <c r="M7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -7605,8 +7358,14 @@
       <c r="M8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -7646,8 +7405,14 @@
       <c r="M9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -7687,8 +7452,14 @@
       <c r="M10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7728,8 +7499,14 @@
       <c r="M11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -7769,8 +7546,14 @@
       <c r="M12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>6</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -7810,8 +7593,14 @@
       <c r="M13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>6</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -7851,8 +7640,14 @@
       <c r="M14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -7892,8 +7687,14 @@
       <c r="M15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>6</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -7933,8 +7734,14 @@
       <c r="M16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -7974,8 +7781,14 @@
       <c r="M17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -8015,8 +7828,14 @@
       <c r="M18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>6</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -8056,8 +7875,14 @@
       <c r="M19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>6</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -8097,8 +7922,14 @@
       <c r="M20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -8138,8 +7969,14 @@
       <c r="M21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>6</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -8179,8 +8016,14 @@
       <c r="M22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>6</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -8220,8 +8063,14 @@
       <c r="M23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>6</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -8261,8 +8110,14 @@
       <c r="M24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -8300,6 +8155,12 @@
         <v>0</v>
       </c>
       <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>6</v>
+      </c>
+      <c r="O25">
         <v>2</v>
       </c>
     </row>

</xml_diff>